<commit_message>
Agente Random y graficos de Performance por porcentaje de suciedad
</commit_message>
<xml_diff>
--- a/tp2-agentes-racionales/code/agente_reflexivo_resultados.xlsx
+++ b/tp2-agentes-racionales/code/agente_reflexivo_resultados.xlsx
@@ -468,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -516,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -628,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -708,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -785,10 +785,10 @@
         <v>0.4</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>14</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="23">
@@ -804,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -817,10 +817,10 @@
         <v>0.4</v>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>13</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25">
@@ -833,10 +833,10 @@
         <v>0.4</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>1000</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
@@ -849,10 +849,10 @@
         <v>0.4</v>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="27">
@@ -868,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -900,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
@@ -916,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -980,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35">
@@ -993,10 +993,10 @@
         <v>0.8</v>
       </c>
       <c r="C35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
-        <v>1000</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36">
@@ -1028,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1041,10 +1041,10 @@
         <v>0.8</v>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
-        <v>1000</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39">
@@ -1076,7 +1076,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41">
@@ -1089,10 +1089,10 @@
         <v>0.8</v>
       </c>
       <c r="C41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="42">
@@ -1108,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43">
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44">
@@ -1140,7 +1140,7 @@
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45">
@@ -1156,7 +1156,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>158</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46">
@@ -1172,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47">
@@ -1188,7 +1188,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
@@ -1204,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49">
@@ -1220,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50">
@@ -1236,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>53</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51">
@@ -1252,7 +1252,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52">
@@ -1268,7 +1268,7 @@
         <v>3</v>
       </c>
       <c r="D52" t="n">
-        <v>25</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53">
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="D53" t="n">
-        <v>148</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54">
@@ -1297,10 +1297,10 @@
         <v>0.2</v>
       </c>
       <c r="C54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D54" t="n">
-        <v>13</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="55">
@@ -1316,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="D55" t="n">
-        <v>50</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56">
@@ -1348,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="D57" t="n">
-        <v>11</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58">
@@ -1364,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="D58" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59">
@@ -1377,10 +1377,10 @@
         <v>0.2</v>
       </c>
       <c r="C59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" t="n">
-        <v>1000</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60">
@@ -1396,7 +1396,7 @@
         <v>3</v>
       </c>
       <c r="D60" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61">
@@ -1412,7 +1412,7 @@
         <v>3</v>
       </c>
       <c r="D61" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62">
@@ -1425,7 +1425,7 @@
         <v>0.4</v>
       </c>
       <c r="C62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D62" t="n">
         <v>1000</v>
@@ -1441,10 +1441,10 @@
         <v>0.4</v>
       </c>
       <c r="C63" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>1000</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64">
@@ -1457,10 +1457,10 @@
         <v>0.4</v>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" t="n">
-        <v>73</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="65">
@@ -1473,10 +1473,10 @@
         <v>0.4</v>
       </c>
       <c r="C65" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>1000</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66">
@@ -1489,7 +1489,7 @@
         <v>0.4</v>
       </c>
       <c r="C66" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D66" t="n">
         <v>1000</v>
@@ -1505,10 +1505,10 @@
         <v>0.4</v>
       </c>
       <c r="C67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D67" t="n">
-        <v>94</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="68">
@@ -1521,7 +1521,7 @@
         <v>0.4</v>
       </c>
       <c r="C68" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68" t="n">
         <v>1000</v>
@@ -1553,7 +1553,7 @@
         <v>0.4</v>
       </c>
       <c r="C70" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D70" t="n">
         <v>1000</v>
@@ -1569,10 +1569,10 @@
         <v>0.4</v>
       </c>
       <c r="C71" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D71" t="n">
-        <v>47</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="72">
@@ -1601,7 +1601,7 @@
         <v>0.8</v>
       </c>
       <c r="C73" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D73" t="n">
         <v>1000</v>
@@ -1617,7 +1617,7 @@
         <v>0.8</v>
       </c>
       <c r="C74" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D74" t="n">
         <v>1000</v>
@@ -1633,7 +1633,7 @@
         <v>0.8</v>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D75" t="n">
         <v>1000</v>
@@ -1649,7 +1649,7 @@
         <v>0.8</v>
       </c>
       <c r="C76" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D76" t="n">
         <v>1000</v>
@@ -1665,7 +1665,7 @@
         <v>0.8</v>
       </c>
       <c r="C77" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D77" t="n">
         <v>1000</v>
@@ -1681,7 +1681,7 @@
         <v>0.8</v>
       </c>
       <c r="C78" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D78" t="n">
         <v>1000</v>
@@ -1697,7 +1697,7 @@
         <v>0.8</v>
       </c>
       <c r="C79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D79" t="n">
         <v>1000</v>
@@ -1713,7 +1713,7 @@
         <v>0.8</v>
       </c>
       <c r="C80" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D80" t="n">
         <v>1000</v>
@@ -1729,7 +1729,7 @@
         <v>0.8</v>
       </c>
       <c r="C81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D81" t="n">
         <v>1000</v>
@@ -1745,10 +1745,10 @@
         <v>0.1</v>
       </c>
       <c r="C82" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D82" t="n">
-        <v>1000</v>
+        <v>496</v>
       </c>
     </row>
     <row r="83">
@@ -1761,10 +1761,10 @@
         <v>0.1</v>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D83" t="n">
-        <v>136</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="84">
@@ -1777,10 +1777,10 @@
         <v>0.1</v>
       </c>
       <c r="C84" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D84" t="n">
-        <v>1000</v>
+        <v>365</v>
       </c>
     </row>
     <row r="85">
@@ -1796,7 +1796,7 @@
         <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>470</v>
+        <v>913</v>
       </c>
     </row>
     <row r="86">
@@ -1812,7 +1812,7 @@
         <v>6</v>
       </c>
       <c r="D86" t="n">
-        <v>475</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87">
@@ -1825,10 +1825,10 @@
         <v>0.1</v>
       </c>
       <c r="C87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D87" t="n">
-        <v>178</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="88">
@@ -1841,10 +1841,10 @@
         <v>0.1</v>
       </c>
       <c r="C88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D88" t="n">
-        <v>131</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="89">
@@ -1873,10 +1873,10 @@
         <v>0.1</v>
       </c>
       <c r="C90" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D90" t="n">
-        <v>1000</v>
+        <v>257</v>
       </c>
     </row>
     <row r="91">
@@ -1889,10 +1889,10 @@
         <v>0.1</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D91" t="n">
-        <v>1000</v>
+        <v>380</v>
       </c>
     </row>
     <row r="92">
@@ -1908,7 +1908,7 @@
         <v>13</v>
       </c>
       <c r="D92" t="n">
-        <v>753</v>
+        <v>843</v>
       </c>
     </row>
     <row r="93">
@@ -1921,7 +1921,7 @@
         <v>0.2</v>
       </c>
       <c r="C93" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D93" t="n">
         <v>1000</v>
@@ -1953,7 +1953,7 @@
         <v>0.2</v>
       </c>
       <c r="C95" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D95" t="n">
         <v>1000</v>
@@ -1969,10 +1969,10 @@
         <v>0.2</v>
       </c>
       <c r="C96" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D96" t="n">
-        <v>340</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="97">
@@ -2017,7 +2017,7 @@
         <v>0.2</v>
       </c>
       <c r="C99" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D99" t="n">
         <v>1000</v>
@@ -2033,10 +2033,10 @@
         <v>0.2</v>
       </c>
       <c r="C100" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D100" t="n">
-        <v>533</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="101">
@@ -2049,7 +2049,7 @@
         <v>0.2</v>
       </c>
       <c r="C101" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D101" t="n">
         <v>1000</v>
@@ -2081,7 +2081,7 @@
         <v>0.4</v>
       </c>
       <c r="C103" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D103" t="n">
         <v>1000</v>
@@ -2097,7 +2097,7 @@
         <v>0.4</v>
       </c>
       <c r="C104" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D104" t="n">
         <v>1000</v>
@@ -2113,7 +2113,7 @@
         <v>0.4</v>
       </c>
       <c r="C105" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D105" t="n">
         <v>1000</v>
@@ -2129,7 +2129,7 @@
         <v>0.4</v>
       </c>
       <c r="C106" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D106" t="n">
         <v>1000</v>
@@ -2145,7 +2145,7 @@
         <v>0.4</v>
       </c>
       <c r="C107" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D107" t="n">
         <v>1000</v>
@@ -2161,7 +2161,7 @@
         <v>0.4</v>
       </c>
       <c r="C108" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D108" t="n">
         <v>1000</v>
@@ -2177,7 +2177,7 @@
         <v>0.4</v>
       </c>
       <c r="C109" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D109" t="n">
         <v>1000</v>
@@ -2193,7 +2193,7 @@
         <v>0.4</v>
       </c>
       <c r="C110" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D110" t="n">
         <v>1000</v>
@@ -2209,7 +2209,7 @@
         <v>0.4</v>
       </c>
       <c r="C111" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D111" t="n">
         <v>1000</v>
@@ -2225,7 +2225,7 @@
         <v>0.8</v>
       </c>
       <c r="C112" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D112" t="n">
         <v>1000</v>
@@ -2241,7 +2241,7 @@
         <v>0.8</v>
       </c>
       <c r="C113" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D113" t="n">
         <v>1000</v>
@@ -2257,7 +2257,7 @@
         <v>0.8</v>
       </c>
       <c r="C114" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D114" t="n">
         <v>1000</v>
@@ -2273,7 +2273,7 @@
         <v>0.8</v>
       </c>
       <c r="C115" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D115" t="n">
         <v>1000</v>
@@ -2289,7 +2289,7 @@
         <v>0.8</v>
       </c>
       <c r="C116" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D116" t="n">
         <v>1000</v>
@@ -2305,7 +2305,7 @@
         <v>0.8</v>
       </c>
       <c r="C117" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D117" t="n">
         <v>1000</v>
@@ -2321,7 +2321,7 @@
         <v>0.8</v>
       </c>
       <c r="C118" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D118" t="n">
         <v>1000</v>
@@ -2337,7 +2337,7 @@
         <v>0.8</v>
       </c>
       <c r="C119" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D119" t="n">
         <v>1000</v>
@@ -2353,7 +2353,7 @@
         <v>0.8</v>
       </c>
       <c r="C120" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D120" t="n">
         <v>1000</v>
@@ -2369,7 +2369,7 @@
         <v>0.8</v>
       </c>
       <c r="C121" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D121" t="n">
         <v>1000</v>
@@ -2385,7 +2385,7 @@
         <v>0.1</v>
       </c>
       <c r="C122" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D122" t="n">
         <v>1000</v>
@@ -2401,7 +2401,7 @@
         <v>0.1</v>
       </c>
       <c r="C123" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D123" t="n">
         <v>1000</v>
@@ -2417,7 +2417,7 @@
         <v>0.1</v>
       </c>
       <c r="C124" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D124" t="n">
         <v>1000</v>
@@ -2433,7 +2433,7 @@
         <v>0.1</v>
       </c>
       <c r="C125" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D125" t="n">
         <v>1000</v>
@@ -2449,7 +2449,7 @@
         <v>0.1</v>
       </c>
       <c r="C126" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D126" t="n">
         <v>1000</v>
@@ -2465,7 +2465,7 @@
         <v>0.1</v>
       </c>
       <c r="C127" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D127" t="n">
         <v>1000</v>
@@ -2481,7 +2481,7 @@
         <v>0.1</v>
       </c>
       <c r="C128" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D128" t="n">
         <v>1000</v>
@@ -2497,7 +2497,7 @@
         <v>0.1</v>
       </c>
       <c r="C129" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D129" t="n">
         <v>1000</v>
@@ -2513,7 +2513,7 @@
         <v>0.1</v>
       </c>
       <c r="C130" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D130" t="n">
         <v>1000</v>
@@ -2529,7 +2529,7 @@
         <v>0.1</v>
       </c>
       <c r="C131" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D131" t="n">
         <v>1000</v>
@@ -2545,7 +2545,7 @@
         <v>0.2</v>
       </c>
       <c r="C132" t="n">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D132" t="n">
         <v>1000</v>
@@ -2561,7 +2561,7 @@
         <v>0.2</v>
       </c>
       <c r="C133" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D133" t="n">
         <v>1000</v>
@@ -2577,7 +2577,7 @@
         <v>0.2</v>
       </c>
       <c r="C134" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D134" t="n">
         <v>1000</v>
@@ -2593,7 +2593,7 @@
         <v>0.2</v>
       </c>
       <c r="C135" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D135" t="n">
         <v>1000</v>
@@ -2609,7 +2609,7 @@
         <v>0.2</v>
       </c>
       <c r="C136" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D136" t="n">
         <v>1000</v>
@@ -2625,7 +2625,7 @@
         <v>0.2</v>
       </c>
       <c r="C137" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D137" t="n">
         <v>1000</v>
@@ -2641,7 +2641,7 @@
         <v>0.2</v>
       </c>
       <c r="C138" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D138" t="n">
         <v>1000</v>
@@ -2657,7 +2657,7 @@
         <v>0.2</v>
       </c>
       <c r="C139" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D139" t="n">
         <v>1000</v>
@@ -2673,7 +2673,7 @@
         <v>0.2</v>
       </c>
       <c r="C140" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D140" t="n">
         <v>1000</v>
@@ -2689,7 +2689,7 @@
         <v>0.2</v>
       </c>
       <c r="C141" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D141" t="n">
         <v>1000</v>
@@ -2705,7 +2705,7 @@
         <v>0.4</v>
       </c>
       <c r="C142" t="n">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D142" t="n">
         <v>1000</v>
@@ -2721,7 +2721,7 @@
         <v>0.4</v>
       </c>
       <c r="C143" t="n">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D143" t="n">
         <v>1000</v>
@@ -2737,7 +2737,7 @@
         <v>0.4</v>
       </c>
       <c r="C144" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D144" t="n">
         <v>1000</v>
@@ -2753,7 +2753,7 @@
         <v>0.4</v>
       </c>
       <c r="C145" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D145" t="n">
         <v>1000</v>
@@ -2769,7 +2769,7 @@
         <v>0.4</v>
       </c>
       <c r="C146" t="n">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D146" t="n">
         <v>1000</v>
@@ -2785,7 +2785,7 @@
         <v>0.4</v>
       </c>
       <c r="C147" t="n">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D147" t="n">
         <v>1000</v>
@@ -2801,7 +2801,7 @@
         <v>0.4</v>
       </c>
       <c r="C148" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D148" t="n">
         <v>1000</v>
@@ -2817,7 +2817,7 @@
         <v>0.4</v>
       </c>
       <c r="C149" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D149" t="n">
         <v>1000</v>
@@ -2833,7 +2833,7 @@
         <v>0.4</v>
       </c>
       <c r="C150" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D150" t="n">
         <v>1000</v>
@@ -2849,7 +2849,7 @@
         <v>0.4</v>
       </c>
       <c r="C151" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D151" t="n">
         <v>1000</v>
@@ -2865,7 +2865,7 @@
         <v>0.8</v>
       </c>
       <c r="C152" t="n">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D152" t="n">
         <v>1000</v>
@@ -2881,7 +2881,7 @@
         <v>0.8</v>
       </c>
       <c r="C153" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D153" t="n">
         <v>1000</v>
@@ -2897,7 +2897,7 @@
         <v>0.8</v>
       </c>
       <c r="C154" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D154" t="n">
         <v>1000</v>
@@ -2913,7 +2913,7 @@
         <v>0.8</v>
       </c>
       <c r="C155" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D155" t="n">
         <v>1000</v>
@@ -2929,7 +2929,7 @@
         <v>0.8</v>
       </c>
       <c r="C156" t="n">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D156" t="n">
         <v>1000</v>
@@ -2945,7 +2945,7 @@
         <v>0.8</v>
       </c>
       <c r="C157" t="n">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D157" t="n">
         <v>1000</v>
@@ -2961,7 +2961,7 @@
         <v>0.8</v>
       </c>
       <c r="C158" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D158" t="n">
         <v>1000</v>
@@ -2977,7 +2977,7 @@
         <v>0.8</v>
       </c>
       <c r="C159" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D159" t="n">
         <v>1000</v>
@@ -2993,7 +2993,7 @@
         <v>0.8</v>
       </c>
       <c r="C160" t="n">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D160" t="n">
         <v>1000</v>
@@ -3009,7 +3009,7 @@
         <v>0.8</v>
       </c>
       <c r="C161" t="n">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="D161" t="n">
         <v>1000</v>
@@ -3025,7 +3025,7 @@
         <v>0.1</v>
       </c>
       <c r="C162" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D162" t="n">
         <v>1000</v>
@@ -3041,7 +3041,7 @@
         <v>0.1</v>
       </c>
       <c r="C163" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D163" t="n">
         <v>1000</v>
@@ -3057,7 +3057,7 @@
         <v>0.1</v>
       </c>
       <c r="C164" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D164" t="n">
         <v>1000</v>
@@ -3073,7 +3073,7 @@
         <v>0.1</v>
       </c>
       <c r="C165" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D165" t="n">
         <v>1000</v>
@@ -3089,7 +3089,7 @@
         <v>0.1</v>
       </c>
       <c r="C166" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D166" t="n">
         <v>1000</v>
@@ -3105,7 +3105,7 @@
         <v>0.1</v>
       </c>
       <c r="C167" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D167" t="n">
         <v>1000</v>
@@ -3121,7 +3121,7 @@
         <v>0.1</v>
       </c>
       <c r="C168" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D168" t="n">
         <v>1000</v>
@@ -3137,7 +3137,7 @@
         <v>0.1</v>
       </c>
       <c r="C169" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D169" t="n">
         <v>1000</v>
@@ -3153,7 +3153,7 @@
         <v>0.1</v>
       </c>
       <c r="C170" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D170" t="n">
         <v>1000</v>
@@ -3169,7 +3169,7 @@
         <v>0.1</v>
       </c>
       <c r="C171" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D171" t="n">
         <v>1000</v>
@@ -3185,7 +3185,7 @@
         <v>0.2</v>
       </c>
       <c r="C172" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D172" t="n">
         <v>1000</v>
@@ -3201,7 +3201,7 @@
         <v>0.2</v>
       </c>
       <c r="C173" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D173" t="n">
         <v>1000</v>
@@ -3217,7 +3217,7 @@
         <v>0.2</v>
       </c>
       <c r="C174" t="n">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D174" t="n">
         <v>1000</v>
@@ -3233,7 +3233,7 @@
         <v>0.2</v>
       </c>
       <c r="C175" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D175" t="n">
         <v>1000</v>
@@ -3249,7 +3249,7 @@
         <v>0.2</v>
       </c>
       <c r="C176" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D176" t="n">
         <v>1000</v>
@@ -3265,7 +3265,7 @@
         <v>0.2</v>
       </c>
       <c r="C177" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D177" t="n">
         <v>1000</v>
@@ -3281,7 +3281,7 @@
         <v>0.2</v>
       </c>
       <c r="C178" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D178" t="n">
         <v>1000</v>
@@ -3297,7 +3297,7 @@
         <v>0.2</v>
       </c>
       <c r="C179" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D179" t="n">
         <v>1000</v>
@@ -3313,7 +3313,7 @@
         <v>0.2</v>
       </c>
       <c r="C180" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D180" t="n">
         <v>1000</v>
@@ -3329,7 +3329,7 @@
         <v>0.2</v>
       </c>
       <c r="C181" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D181" t="n">
         <v>1000</v>
@@ -3345,7 +3345,7 @@
         <v>0.4</v>
       </c>
       <c r="C182" t="n">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D182" t="n">
         <v>1000</v>
@@ -3361,7 +3361,7 @@
         <v>0.4</v>
       </c>
       <c r="C183" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="D183" t="n">
         <v>1000</v>
@@ -3377,7 +3377,7 @@
         <v>0.4</v>
       </c>
       <c r="C184" t="n">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="D184" t="n">
         <v>1000</v>
@@ -3393,7 +3393,7 @@
         <v>0.4</v>
       </c>
       <c r="C185" t="n">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="D185" t="n">
         <v>1000</v>
@@ -3409,7 +3409,7 @@
         <v>0.4</v>
       </c>
       <c r="C186" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D186" t="n">
         <v>1000</v>
@@ -3425,7 +3425,7 @@
         <v>0.4</v>
       </c>
       <c r="C187" t="n">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="D187" t="n">
         <v>1000</v>
@@ -3441,7 +3441,7 @@
         <v>0.4</v>
       </c>
       <c r="C188" t="n">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D188" t="n">
         <v>1000</v>
@@ -3457,7 +3457,7 @@
         <v>0.4</v>
       </c>
       <c r="C189" t="n">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D189" t="n">
         <v>1000</v>
@@ -3473,7 +3473,7 @@
         <v>0.4</v>
       </c>
       <c r="C190" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D190" t="n">
         <v>1000</v>
@@ -3489,7 +3489,7 @@
         <v>0.4</v>
       </c>
       <c r="C191" t="n">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="D191" t="n">
         <v>1000</v>
@@ -3505,7 +3505,7 @@
         <v>0.8</v>
       </c>
       <c r="C192" t="n">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D192" t="n">
         <v>1000</v>
@@ -3521,7 +3521,7 @@
         <v>0.8</v>
       </c>
       <c r="C193" t="n">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D193" t="n">
         <v>1000</v>
@@ -3537,7 +3537,7 @@
         <v>0.8</v>
       </c>
       <c r="C194" t="n">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="D194" t="n">
         <v>1000</v>
@@ -3553,7 +3553,7 @@
         <v>0.8</v>
       </c>
       <c r="C195" t="n">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D195" t="n">
         <v>1000</v>
@@ -3569,7 +3569,7 @@
         <v>0.8</v>
       </c>
       <c r="C196" t="n">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="D196" t="n">
         <v>1000</v>
@@ -3585,7 +3585,7 @@
         <v>0.8</v>
       </c>
       <c r="C197" t="n">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="D197" t="n">
         <v>1000</v>
@@ -3601,7 +3601,7 @@
         <v>0.8</v>
       </c>
       <c r="C198" t="n">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="D198" t="n">
         <v>1000</v>
@@ -3617,7 +3617,7 @@
         <v>0.8</v>
       </c>
       <c r="C199" t="n">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="D199" t="n">
         <v>1000</v>
@@ -3633,7 +3633,7 @@
         <v>0.8</v>
       </c>
       <c r="C200" t="n">
-        <v>197</v>
+        <v>142</v>
       </c>
       <c r="D200" t="n">
         <v>1000</v>
@@ -3649,7 +3649,7 @@
         <v>0.8</v>
       </c>
       <c r="C201" t="n">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="D201" t="n">
         <v>1000</v>
@@ -3665,7 +3665,7 @@
         <v>0.1</v>
       </c>
       <c r="C202" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D202" t="n">
         <v>1000</v>
@@ -3681,7 +3681,7 @@
         <v>0.1</v>
       </c>
       <c r="C203" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D203" t="n">
         <v>1000</v>
@@ -3697,7 +3697,7 @@
         <v>0.1</v>
       </c>
       <c r="C204" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D204" t="n">
         <v>1000</v>
@@ -3713,7 +3713,7 @@
         <v>0.1</v>
       </c>
       <c r="C205" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D205" t="n">
         <v>1000</v>
@@ -3729,7 +3729,7 @@
         <v>0.1</v>
       </c>
       <c r="C206" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D206" t="n">
         <v>1000</v>
@@ -3745,7 +3745,7 @@
         <v>0.1</v>
       </c>
       <c r="C207" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D207" t="n">
         <v>1000</v>
@@ -3761,7 +3761,7 @@
         <v>0.1</v>
       </c>
       <c r="C208" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D208" t="n">
         <v>1000</v>
@@ -3777,7 +3777,7 @@
         <v>0.1</v>
       </c>
       <c r="C209" t="n">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D209" t="n">
         <v>1000</v>
@@ -3793,7 +3793,7 @@
         <v>0.1</v>
       </c>
       <c r="C210" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D210" t="n">
         <v>1000</v>
@@ -3809,7 +3809,7 @@
         <v>0.1</v>
       </c>
       <c r="C211" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D211" t="n">
         <v>1000</v>
@@ -3825,7 +3825,7 @@
         <v>0.2</v>
       </c>
       <c r="C212" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D212" t="n">
         <v>1000</v>
@@ -3841,7 +3841,7 @@
         <v>0.2</v>
       </c>
       <c r="C213" t="n">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D213" t="n">
         <v>1000</v>
@@ -3857,7 +3857,7 @@
         <v>0.2</v>
       </c>
       <c r="C214" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D214" t="n">
         <v>1000</v>
@@ -3873,7 +3873,7 @@
         <v>0.2</v>
       </c>
       <c r="C215" t="n">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D215" t="n">
         <v>1000</v>
@@ -3889,7 +3889,7 @@
         <v>0.2</v>
       </c>
       <c r="C216" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D216" t="n">
         <v>1000</v>
@@ -3905,7 +3905,7 @@
         <v>0.2</v>
       </c>
       <c r="C217" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D217" t="n">
         <v>1000</v>
@@ -3921,7 +3921,7 @@
         <v>0.2</v>
       </c>
       <c r="C218" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D218" t="n">
         <v>1000</v>
@@ -3937,7 +3937,7 @@
         <v>0.2</v>
       </c>
       <c r="C219" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D219" t="n">
         <v>1000</v>
@@ -3953,7 +3953,7 @@
         <v>0.2</v>
       </c>
       <c r="C220" t="n">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D220" t="n">
         <v>1000</v>
@@ -3969,7 +3969,7 @@
         <v>0.2</v>
       </c>
       <c r="C221" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D221" t="n">
         <v>1000</v>
@@ -3985,7 +3985,7 @@
         <v>0.4</v>
       </c>
       <c r="C222" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D222" t="n">
         <v>1000</v>
@@ -4001,7 +4001,7 @@
         <v>0.4</v>
       </c>
       <c r="C223" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D223" t="n">
         <v>1000</v>
@@ -4017,7 +4017,7 @@
         <v>0.4</v>
       </c>
       <c r="C224" t="n">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D224" t="n">
         <v>1000</v>
@@ -4033,7 +4033,7 @@
         <v>0.4</v>
       </c>
       <c r="C225" t="n">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D225" t="n">
         <v>1000</v>
@@ -4049,7 +4049,7 @@
         <v>0.4</v>
       </c>
       <c r="C226" t="n">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="D226" t="n">
         <v>1000</v>
@@ -4065,7 +4065,7 @@
         <v>0.4</v>
       </c>
       <c r="C227" t="n">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D227" t="n">
         <v>1000</v>
@@ -4081,7 +4081,7 @@
         <v>0.4</v>
       </c>
       <c r="C228" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D228" t="n">
         <v>1000</v>
@@ -4097,7 +4097,7 @@
         <v>0.4</v>
       </c>
       <c r="C229" t="n">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D229" t="n">
         <v>1000</v>
@@ -4113,7 +4113,7 @@
         <v>0.4</v>
       </c>
       <c r="C230" t="n">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D230" t="n">
         <v>1000</v>
@@ -4129,7 +4129,7 @@
         <v>0.4</v>
       </c>
       <c r="C231" t="n">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D231" t="n">
         <v>1000</v>
@@ -4145,7 +4145,7 @@
         <v>0.8</v>
       </c>
       <c r="C232" t="n">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D232" t="n">
         <v>1000</v>
@@ -4161,7 +4161,7 @@
         <v>0.8</v>
       </c>
       <c r="C233" t="n">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D233" t="n">
         <v>1000</v>
@@ -4177,7 +4177,7 @@
         <v>0.8</v>
       </c>
       <c r="C234" t="n">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="D234" t="n">
         <v>1000</v>
@@ -4193,7 +4193,7 @@
         <v>0.8</v>
       </c>
       <c r="C235" t="n">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D235" t="n">
         <v>1000</v>
@@ -4209,7 +4209,7 @@
         <v>0.8</v>
       </c>
       <c r="C236" t="n">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="D236" t="n">
         <v>1000</v>
@@ -4225,7 +4225,7 @@
         <v>0.8</v>
       </c>
       <c r="C237" t="n">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D237" t="n">
         <v>1000</v>
@@ -4241,7 +4241,7 @@
         <v>0.8</v>
       </c>
       <c r="C238" t="n">
-        <v>189</v>
+        <v>143</v>
       </c>
       <c r="D238" t="n">
         <v>1000</v>
@@ -4257,7 +4257,7 @@
         <v>0.8</v>
       </c>
       <c r="C239" t="n">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="D239" t="n">
         <v>1000</v>
@@ -4273,7 +4273,7 @@
         <v>0.8</v>
       </c>
       <c r="C240" t="n">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D240" t="n">
         <v>1000</v>
@@ -4289,7 +4289,7 @@
         <v>0.8</v>
       </c>
       <c r="C241" t="n">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="D241" t="n">
         <v>1000</v>
@@ -4305,7 +4305,7 @@
         <v>0.1</v>
       </c>
       <c r="C242" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D242" t="n">
         <v>1000</v>
@@ -4321,7 +4321,7 @@
         <v>0.1</v>
       </c>
       <c r="C243" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D243" t="n">
         <v>1000</v>
@@ -4337,7 +4337,7 @@
         <v>0.1</v>
       </c>
       <c r="C244" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D244" t="n">
         <v>1000</v>
@@ -4353,7 +4353,7 @@
         <v>0.1</v>
       </c>
       <c r="C245" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D245" t="n">
         <v>1000</v>
@@ -4369,7 +4369,7 @@
         <v>0.1</v>
       </c>
       <c r="C246" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D246" t="n">
         <v>1000</v>
@@ -4385,7 +4385,7 @@
         <v>0.1</v>
       </c>
       <c r="C247" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D247" t="n">
         <v>1000</v>
@@ -4401,7 +4401,7 @@
         <v>0.1</v>
       </c>
       <c r="C248" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D248" t="n">
         <v>1000</v>
@@ -4417,7 +4417,7 @@
         <v>0.1</v>
       </c>
       <c r="C249" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D249" t="n">
         <v>1000</v>
@@ -4433,7 +4433,7 @@
         <v>0.1</v>
       </c>
       <c r="C250" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D250" t="n">
         <v>1000</v>
@@ -4449,7 +4449,7 @@
         <v>0.1</v>
       </c>
       <c r="C251" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D251" t="n">
         <v>1000</v>
@@ -4465,7 +4465,7 @@
         <v>0.2</v>
       </c>
       <c r="C252" t="n">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="D252" t="n">
         <v>1000</v>
@@ -4481,7 +4481,7 @@
         <v>0.2</v>
       </c>
       <c r="C253" t="n">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D253" t="n">
         <v>1000</v>
@@ -4497,7 +4497,7 @@
         <v>0.2</v>
       </c>
       <c r="C254" t="n">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D254" t="n">
         <v>1000</v>
@@ -4513,7 +4513,7 @@
         <v>0.2</v>
       </c>
       <c r="C255" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D255" t="n">
         <v>1000</v>
@@ -4529,7 +4529,7 @@
         <v>0.2</v>
       </c>
       <c r="C256" t="n">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D256" t="n">
         <v>1000</v>
@@ -4545,7 +4545,7 @@
         <v>0.2</v>
       </c>
       <c r="C257" t="n">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D257" t="n">
         <v>1000</v>
@@ -4561,7 +4561,7 @@
         <v>0.2</v>
       </c>
       <c r="C258" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D258" t="n">
         <v>1000</v>
@@ -4577,7 +4577,7 @@
         <v>0.2</v>
       </c>
       <c r="C259" t="n">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D259" t="n">
         <v>1000</v>
@@ -4593,7 +4593,7 @@
         <v>0.2</v>
       </c>
       <c r="C260" t="n">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D260" t="n">
         <v>1000</v>
@@ -4609,7 +4609,7 @@
         <v>0.2</v>
       </c>
       <c r="C261" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D261" t="n">
         <v>1000</v>
@@ -4625,7 +4625,7 @@
         <v>0.4</v>
       </c>
       <c r="C262" t="n">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D262" t="n">
         <v>1000</v>
@@ -4641,7 +4641,7 @@
         <v>0.4</v>
       </c>
       <c r="C263" t="n">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="D263" t="n">
         <v>1000</v>
@@ -4657,7 +4657,7 @@
         <v>0.4</v>
       </c>
       <c r="C264" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D264" t="n">
         <v>1000</v>
@@ -4673,7 +4673,7 @@
         <v>0.4</v>
       </c>
       <c r="C265" t="n">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="D265" t="n">
         <v>1000</v>
@@ -4689,7 +4689,7 @@
         <v>0.4</v>
       </c>
       <c r="C266" t="n">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="D266" t="n">
         <v>1000</v>
@@ -4705,7 +4705,7 @@
         <v>0.4</v>
       </c>
       <c r="C267" t="n">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D267" t="n">
         <v>1000</v>
@@ -4721,7 +4721,7 @@
         <v>0.4</v>
       </c>
       <c r="C268" t="n">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="D268" t="n">
         <v>1000</v>
@@ -4737,7 +4737,7 @@
         <v>0.4</v>
       </c>
       <c r="C269" t="n">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D269" t="n">
         <v>1000</v>
@@ -4753,7 +4753,7 @@
         <v>0.4</v>
       </c>
       <c r="C270" t="n">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="D270" t="n">
         <v>1000</v>
@@ -4769,7 +4769,7 @@
         <v>0.4</v>
       </c>
       <c r="C271" t="n">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D271" t="n">
         <v>1000</v>
@@ -4785,7 +4785,7 @@
         <v>0.8</v>
       </c>
       <c r="C272" t="n">
-        <v>206</v>
+        <v>162</v>
       </c>
       <c r="D272" t="n">
         <v>1000</v>
@@ -4801,7 +4801,7 @@
         <v>0.8</v>
       </c>
       <c r="C273" t="n">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D273" t="n">
         <v>1000</v>
@@ -4817,7 +4817,7 @@
         <v>0.8</v>
       </c>
       <c r="C274" t="n">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="D274" t="n">
         <v>1000</v>
@@ -4833,7 +4833,7 @@
         <v>0.8</v>
       </c>
       <c r="C275" t="n">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D275" t="n">
         <v>1000</v>
@@ -4849,7 +4849,7 @@
         <v>0.8</v>
       </c>
       <c r="C276" t="n">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="D276" t="n">
         <v>1000</v>
@@ -4865,7 +4865,7 @@
         <v>0.8</v>
       </c>
       <c r="C277" t="n">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D277" t="n">
         <v>1000</v>
@@ -4881,7 +4881,7 @@
         <v>0.8</v>
       </c>
       <c r="C278" t="n">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D278" t="n">
         <v>1000</v>
@@ -4897,7 +4897,7 @@
         <v>0.8</v>
       </c>
       <c r="C279" t="n">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="D279" t="n">
         <v>1000</v>
@@ -4913,7 +4913,7 @@
         <v>0.8</v>
       </c>
       <c r="C280" t="n">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="D280" t="n">
         <v>1000</v>
@@ -4929,7 +4929,7 @@
         <v>0.8</v>
       </c>
       <c r="C281" t="n">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D281" t="n">
         <v>1000</v>

</xml_diff>